<commit_message>
Update Keypad safe worst timing.xlsx
</commit_message>
<xml_diff>
--- a/Keypad safe worst timing.xlsx
+++ b/Keypad safe worst timing.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>combination length</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>after initial 20s</t>
+  </si>
+  <si>
+    <t>combined</t>
   </si>
   <si>
     <t>seconds</t>
@@ -41,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -51,7 +54,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -67,14 +69,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -304,57 +303,64 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>3.0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>10^A2</f>
         <v>1000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <f>C2-3</f>
         <v>997</v>
+      </c>
+      <c r="E2" s="2">
+        <f>D2/A2</f>
+        <v>332.3333333</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
-        <f>(D2*280) +20</f>
-        <v>279180</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="A6" s="2">
+        <f>(E2*288) +20</f>
+        <v>95732</v>
+      </c>
+      <c r="C6" s="2">
         <f>A6/60</f>
-        <v>4653</v>
-      </c>
-      <c r="E6" s="3">
+        <v>1595.533333</v>
+      </c>
+      <c r="E6" s="2">
         <f>C6/60</f>
-        <v>77.55</v>
-      </c>
-      <c r="G6" s="3">
+        <v>26.59222222</v>
+      </c>
+      <c r="G6" s="2">
         <f>E6/24</f>
-        <v>3.23125</v>
-      </c>
-      <c r="I6" s="3">
+        <v>1.108009259</v>
+      </c>
+      <c r="I6" s="2">
         <f>G6/365</f>
-        <v>0.008852739726</v>
+        <v>0.003035641806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>